<commit_message>
convert Euroto US1178, add Bambu X1-Carbon printer and WPP cost to compare.
</commit_message>
<xml_diff>
--- a/QuotingSheet.xlsx
+++ b/QuotingSheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stuff\YouTube\43_PrintCosts\Calc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awv\Documents\XL\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDD617D-EBC0-413C-BB26-BF3BF182BF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9390"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quote" sheetId="1" r:id="rId1"/>
@@ -17,17 +18,28 @@
     <sheet name="Materials" sheetId="3" r:id="rId3"/>
     <sheet name="General" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -77,9 +89,6 @@
     <t>Money unit</t>
   </si>
   <si>
-    <t>€</t>
-  </si>
-  <si>
     <t>Customer</t>
   </si>
   <si>
@@ -170,12 +179,6 @@
     <t>Markup</t>
   </si>
   <si>
-    <t>Suggested prize</t>
-  </si>
-  <si>
-    <t>Quoted prize</t>
-  </si>
-  <si>
     <t>Summary</t>
   </si>
   <si>
@@ -234,16 +237,29 @@
   </si>
   <si>
     <t>Proto Pasta HT-PLA</t>
+  </si>
+  <si>
+    <t>Bambu X1-Carbon</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>Suggested price</t>
+  </si>
+  <si>
+    <t>Quoted price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ &quot;$&quot;_-;\-* #,##0.00\ &quot;$&quot;_-;_-* &quot;-&quot;??\ &quot;$&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -421,7 +437,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -433,7 +449,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -442,7 +458,7 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -454,20 +470,17 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -489,10 +502,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Währung" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -510,7 +526,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1051,13 +1067,13 @@
                   <c:v>2.16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2101666666666667</c:v>
+                  <c:v>8.7300000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1555555555555559</c:v>
+                  <c:v>2.101666666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.5</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>7.5</c:v>
@@ -1733,9 +1749,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1773,7 +1789,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1879,7 +1895,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2021,24 +2037,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
@@ -2048,33 +2062,33 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="G2" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="37"/>
+      <c r="A2" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="G2" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="36"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="31"/>
-      <c r="G3" s="34" t="str">
+        <v>16</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="G3" s="33" t="str">
         <f>B10</f>
         <v>das Filament - PLA - black</v>
       </c>
-      <c r="H3" s="35"/>
+      <c r="H3" s="34"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="11">
         <v>43016</v>
@@ -2084,34 +2098,34 @@
         <v>108</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
+        <v>18</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
       <c r="G5" s="7">
         <f>D12</f>
         <v>8.0833333333333339</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G6" s="8">
         <f>B43</f>
-        <v>33.867441666666664</v>
+        <v>29.450795000000006</v>
       </c>
       <c r="H6" s="6" t="str">
         <f>General!$B$5&amp;" || suggested price"</f>
-        <v>€ || suggested price</v>
+        <v>$ || suggested price</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2121,228 +2135,228 @@
       </c>
       <c r="H7" s="10" t="str">
         <f>General!$B$5&amp;" || quoted"</f>
-        <v>€ || quoted</v>
+        <v>$ || quoted</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
+      <c r="A8" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="33"/>
+        <v>40</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="32"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="33"/>
+      <c r="C10" s="32"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="12">
         <v>108</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="14">
         <f>(B11/VLOOKUP(B10,Materials!A2:I100,5,FALSE))*4/(VLOOKUP(B10,Materials!A2:I100,2,FALSE)^2*PI())</f>
         <v>36.210630897010553</v>
       </c>
       <c r="E11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="14">
         <f>LEFT(B12,FIND(":",B12)-1)+RIGHT(B12,LEN(B12)-FIND(":",B12))/60</f>
         <v>8.0833333333333339</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
+      <c r="A14" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="12">
         <v>0</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="12">
         <v>5</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="12">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="12">
         <v>5</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="21">
         <f>SUM(B15:B18)</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
+      <c r="A21" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="12">
         <v>5</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="12">
         <v>0</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" s="12">
         <v>10</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B25" s="21">
         <f>SUM(B22:B24)</f>
         <v>15</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C26" s="4"/>
     </row>
     <row r="27" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
+      <c r="A27" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" s="12">
         <v>1</v>
       </c>
       <c r="C28" s="4" t="str">
         <f>General!B5</f>
-        <v>€</v>
+        <v>$</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C29" s="4"/>
     </row>
     <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
+      <c r="A31" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B32" s="18">
         <f>B11/1000*VLOOKUP(B10,Materials!A2:I100,9,FALSE)</f>
@@ -2350,53 +2364,51 @@
       </c>
       <c r="C32" s="4" t="str">
         <f>General!$B$5</f>
-        <v>€</v>
-      </c>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
+        <v>$</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B33" s="18">
         <f>D12*VLOOKUP(B9,Printers!A2:G100,6,FALSE)*General!B2</f>
-        <v>0.2101666666666667</v>
+        <v>8.7300000000000003E-2</v>
       </c>
       <c r="C33" s="4" t="str">
         <f>General!$B$5</f>
-        <v>€</v>
+        <v>$</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B34" s="18">
         <f>D12*VLOOKUP(B9,Printers!A2:G100,7,FALSE)</f>
-        <v>2.1555555555555559</v>
+        <v>2.101666666666667</v>
       </c>
       <c r="C34" s="4" t="str">
         <f>General!$B$5</f>
-        <v>€</v>
+        <v>$</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B35" s="18">
         <f>B19/60*General!B3</f>
-        <v>7.5</v>
+        <v>5</v>
       </c>
       <c r="C35" s="4" t="str">
         <f>General!$B$5</f>
-        <v>€</v>
+        <v>$</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" s="18">
         <f>B25/60*General!B3</f>
@@ -2404,12 +2416,12 @@
       </c>
       <c r="C36" s="4" t="str">
         <f>General!$B$5</f>
-        <v>€</v>
+        <v>$</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37" s="18">
         <f>B28</f>
@@ -2417,45 +2429,45 @@
       </c>
       <c r="C37" s="4" t="str">
         <f>General!$B$5</f>
-        <v>€</v>
+        <v>$</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B38" s="17">
         <f>SUM(B32:B37)</f>
-        <v>20.525722222222221</v>
+        <v>17.848966666666669</v>
       </c>
       <c r="C38" s="4" t="str">
         <f>General!$B$5</f>
-        <v>€</v>
+        <v>$</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B39" s="17">
         <f>B38*(General!B4/100+1)</f>
-        <v>22.578294444444445</v>
+        <v>19.633863333333338</v>
       </c>
       <c r="C39" s="4" t="str">
         <f>General!$B$5</f>
-        <v>€</v>
+        <v>$</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="B41" s="32"/>
-      <c r="C41" s="32"/>
+      <c r="A41" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42" s="16">
         <v>1.5</v>
@@ -2463,27 +2475,27 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="B43" s="17">
         <f>B39*B42</f>
-        <v>33.867441666666664</v>
+        <v>29.450795000000006</v>
       </c>
       <c r="C43" s="4" t="str">
         <f>General!$B$5</f>
-        <v>€</v>
+        <v>$</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="B44" s="19">
         <v>33.869999999999997</v>
       </c>
       <c r="C44" s="4" t="str">
         <f>General!$B$5</f>
-        <v>€</v>
+        <v>$</v>
       </c>
     </row>
   </sheetData>
@@ -2511,13 +2523,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Printers!$A$2:$A$100</xm:f>
           </x14:formula1>
           <xm:sqref>B9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Materials!A2:A100</xm:f>
           </x14:formula1>
@@ -2530,14 +2542,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
@@ -2557,21 +2569,21 @@
       </c>
       <c r="C1" s="2" t="str">
         <f>"Price ["&amp;General!B5&amp;"]"</f>
-        <v>Price [€]</v>
+        <v>Price [$]</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="str">
         <f>"Service costs per life ["&amp;General!B5&amp;"]"</f>
-        <v>Service costs per life [€]</v>
+        <v>Service costs per life [$]</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="2" t="str">
         <f>"Depreciation ["&amp;General!B5&amp;"/h]"</f>
-        <v>Depreciation [€/h]</v>
+        <v>Depreciation [$/h]</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2582,20 +2594,20 @@
         <v>1.75</v>
       </c>
       <c r="C2" s="12">
-        <v>450</v>
+        <v>481</v>
       </c>
       <c r="D2" s="12">
         <v>2000</v>
       </c>
       <c r="E2" s="12">
-        <v>100</v>
-      </c>
-      <c r="F2" s="26">
+        <v>107</v>
+      </c>
+      <c r="F2" s="25">
         <v>0.15</v>
       </c>
-      <c r="G2" s="27">
+      <c r="G2" s="26">
         <f>(C2+E2)/D2</f>
-        <v>0.27500000000000002</v>
+        <v>0.29399999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2606,78 +2618,93 @@
         <v>1.75</v>
       </c>
       <c r="C3" s="12">
-        <v>700</v>
+        <v>748</v>
       </c>
       <c r="D3" s="12">
         <v>3000</v>
       </c>
       <c r="E3" s="12">
-        <v>100</v>
-      </c>
-      <c r="F3" s="26">
+        <v>107</v>
+      </c>
+      <c r="F3" s="25">
         <v>0.1</v>
       </c>
-      <c r="G3" s="27">
+      <c r="G3" s="26">
         <f>(C3+E3)/D3</f>
-        <v>0.26666666666666666</v>
+        <v>0.28499999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B4" s="12">
         <v>2.85</v>
       </c>
       <c r="C4" s="12">
-        <v>4400</v>
+        <v>4700</v>
       </c>
       <c r="D4" s="12">
         <v>4000</v>
       </c>
       <c r="E4" s="12">
-        <v>250</v>
-      </c>
-      <c r="F4" s="26">
+        <v>267</v>
+      </c>
+      <c r="F4" s="25">
         <v>0.11</v>
       </c>
-      <c r="G4" s="27">
+      <c r="G4" s="26">
         <f>(C4+E4)/D4</f>
-        <v>1.1625000000000001</v>
+        <v>1.2417499999999999</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B5" s="12">
         <v>2.85</v>
       </c>
       <c r="C5" s="12">
-        <v>5549</v>
+        <v>5928</v>
       </c>
       <c r="D5" s="12">
         <v>5000</v>
       </c>
       <c r="E5" s="12">
-        <v>300</v>
-      </c>
-      <c r="F5" s="26">
+        <v>320</v>
+      </c>
+      <c r="F5" s="25">
         <v>0.12</v>
       </c>
-      <c r="G5" s="27">
+      <c r="G5" s="26">
         <f>(C5+E5)/D5</f>
-        <v>1.1698</v>
+        <v>1.2496</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="25"/>
+      <c r="A6" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="12">
+        <v>1.75</v>
+      </c>
+      <c r="C6" s="12">
+        <v>1600</v>
+      </c>
+      <c r="D6" s="12">
+        <v>10000</v>
+      </c>
+      <c r="E6" s="12">
+        <v>1000</v>
+      </c>
+      <c r="F6" s="25">
+        <v>0.12</v>
+      </c>
+      <c r="G6" s="24">
+        <f>(C6+E6)/D6</f>
+        <v>0.26</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
@@ -2685,8 +2712,8 @@
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="24"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
@@ -2694,8 +2721,8 @@
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="24"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
@@ -2703,8 +2730,8 @@
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="24"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
@@ -2712,8 +2739,8 @@
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="24"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
@@ -2721,8 +2748,8 @@
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="24"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
@@ -2730,8 +2757,8 @@
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="24"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
@@ -2739,8 +2766,8 @@
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="24"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
@@ -2748,8 +2775,8 @@
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="24"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
@@ -2757,8 +2784,8 @@
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="24"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
@@ -2767,7 +2794,7 @@
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
-      <c r="G16" s="25"/>
+      <c r="G16" s="24"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
@@ -2776,7 +2803,7 @@
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
-      <c r="G17" s="25"/>
+      <c r="G17" s="24"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
@@ -2785,7 +2812,7 @@
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
-      <c r="G18" s="25"/>
+      <c r="G18" s="24"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
@@ -2794,7 +2821,7 @@
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
-      <c r="G19" s="25"/>
+      <c r="G19" s="24"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
@@ -2803,7 +2830,7 @@
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
-      <c r="G20" s="25"/>
+      <c r="G20" s="24"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
@@ -2812,7 +2839,7 @@
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
-      <c r="G21" s="25"/>
+      <c r="G21" s="24"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
@@ -2821,7 +2848,7 @@
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
-      <c r="G22" s="25"/>
+      <c r="G22" s="24"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
@@ -2830,7 +2857,7 @@
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
-      <c r="G23" s="25"/>
+      <c r="G23" s="24"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
@@ -2839,7 +2866,7 @@
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
-      <c r="G24" s="25"/>
+      <c r="G24" s="24"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
@@ -2848,7 +2875,7 @@
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
-      <c r="G25" s="25"/>
+      <c r="G25" s="24"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
@@ -2857,7 +2884,7 @@
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
-      <c r="G26" s="25"/>
+      <c r="G26" s="24"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
@@ -2866,7 +2893,7 @@
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
-      <c r="G27" s="25"/>
+      <c r="G27" s="24"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
@@ -2875,7 +2902,7 @@
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
-      <c r="G28" s="25"/>
+      <c r="G28" s="24"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
@@ -2884,7 +2911,7 @@
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
-      <c r="G29" s="25"/>
+      <c r="G29" s="24"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
@@ -2893,7 +2920,7 @@
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
-      <c r="G30" s="25"/>
+      <c r="G30" s="24"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
@@ -2902,7 +2929,7 @@
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
-      <c r="G31" s="25"/>
+      <c r="G31" s="24"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
@@ -2911,7 +2938,7 @@
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
-      <c r="G32" s="25"/>
+      <c r="G32" s="24"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
@@ -2920,7 +2947,7 @@
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
-      <c r="G33" s="25"/>
+      <c r="G33" s="24"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
@@ -2929,7 +2956,7 @@
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
-      <c r="G34" s="25"/>
+      <c r="G34" s="24"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
@@ -2938,7 +2965,7 @@
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
-      <c r="G35" s="25"/>
+      <c r="G35" s="24"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
@@ -2947,7 +2974,7 @@
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
-      <c r="G36" s="25"/>
+      <c r="G36" s="24"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
@@ -2956,7 +2983,7 @@
       <c r="D37" s="12"/>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
-      <c r="G37" s="25"/>
+      <c r="G37" s="24"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
@@ -2965,7 +2992,7 @@
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
-      <c r="G38" s="25"/>
+      <c r="G38" s="24"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
@@ -2974,7 +3001,7 @@
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
-      <c r="G39" s="25"/>
+      <c r="G39" s="24"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
@@ -2983,7 +3010,7 @@
       <c r="D40" s="12"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
-      <c r="G40" s="25"/>
+      <c r="G40" s="24"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
@@ -2992,7 +3019,7 @@
       <c r="D41" s="12"/>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
-      <c r="G41" s="25"/>
+      <c r="G41" s="24"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
@@ -3001,7 +3028,7 @@
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
       <c r="F42" s="12"/>
-      <c r="G42" s="25"/>
+      <c r="G42" s="24"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
@@ -3010,7 +3037,7 @@
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
-      <c r="G43" s="25"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
@@ -3019,7 +3046,7 @@
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
-      <c r="G44" s="25"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
@@ -3028,7 +3055,7 @@
       <c r="D45" s="12"/>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
-      <c r="G45" s="25"/>
+      <c r="G45" s="24"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
@@ -3037,7 +3064,7 @@
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
       <c r="F46" s="12"/>
-      <c r="G46" s="25"/>
+      <c r="G46" s="24"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
@@ -3046,7 +3073,7 @@
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
-      <c r="G47" s="25"/>
+      <c r="G47" s="24"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
@@ -3055,7 +3082,7 @@
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
       <c r="F48" s="12"/>
-      <c r="G48" s="25"/>
+      <c r="G48" s="24"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="12"/>
@@ -3064,7 +3091,7 @@
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
-      <c r="G49" s="25"/>
+      <c r="G49" s="24"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="12"/>
@@ -3073,7 +3100,7 @@
       <c r="D50" s="12"/>
       <c r="E50" s="12"/>
       <c r="F50" s="12"/>
-      <c r="G50" s="25"/>
+      <c r="G50" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3082,14 +3109,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -3112,7 +3139,7 @@
       </c>
       <c r="C1" s="1" t="str">
         <f>"Spool Price ["&amp;General!B5&amp;"]"</f>
-        <v>Spool Price [€]</v>
+        <v>Spool Price [$]</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
@@ -3131,23 +3158,23 @@
       </c>
       <c r="I1" s="1" t="str">
         <f>"Price ["&amp;General!B5&amp;"/kg]"</f>
-        <v>Price [€/kg]</v>
+        <v>Price [$/kg]</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="12">
         <v>1.75</v>
       </c>
-      <c r="C2" s="22">
+      <c r="C2" s="29">
         <v>16</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="22">
         <v>0.8</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="22">
         <v>1.24</v>
       </c>
       <c r="F2" s="12">
@@ -3156,7 +3183,7 @@
       <c r="G2" s="12">
         <v>60</v>
       </c>
-      <c r="H2" s="24">
+      <c r="H2" s="23">
         <f t="shared" ref="H2:H8" si="0">D2/E2*4/(PI()*(B2/100)^2)/10</f>
         <v>268.22689553341149</v>
       </c>
@@ -3167,18 +3194,18 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B3" s="12">
         <v>1.75</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="29">
         <v>45</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="22">
         <v>0.75</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="22">
         <v>1.19</v>
       </c>
       <c r="F3" s="12">
@@ -3187,7 +3214,7 @@
       <c r="G3" s="12">
         <v>80</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="23">
         <f t="shared" si="0"/>
         <v>262.02837483831161</v>
       </c>
@@ -3198,18 +3225,18 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B4" s="12">
         <v>1.75</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="29">
         <v>35</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="22">
         <v>0.5</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="22">
         <v>1.05</v>
       </c>
       <c r="F4" s="12">
@@ -3218,7 +3245,7 @@
       <c r="G4" s="12">
         <v>115</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="23">
         <f t="shared" si="0"/>
         <v>197.97699432227989</v>
       </c>
@@ -3229,18 +3256,18 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B5" s="12">
         <v>1.75</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="29">
         <v>30</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="22">
         <v>1</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="22">
         <v>1.03</v>
       </c>
       <c r="F5" s="12">
@@ -3249,7 +3276,7 @@
       <c r="G5" s="12">
         <v>100</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="23">
         <f t="shared" si="0"/>
         <v>403.64241560853185</v>
       </c>
@@ -3260,18 +3287,18 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B6" s="12">
         <v>1.75</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="29">
         <v>50</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="22">
         <v>0.75</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="22">
         <v>1.27</v>
       </c>
       <c r="F6" s="12">
@@ -3280,7 +3307,7 @@
       <c r="G6" s="12">
         <v>65</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="23">
         <f t="shared" si="0"/>
         <v>245.52265043904791</v>
       </c>
@@ -3291,18 +3318,18 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B7" s="12">
         <v>1.75</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="29">
         <v>22</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="22">
         <v>0.8</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="22">
         <v>1.27</v>
       </c>
       <c r="F7" s="12">
@@ -3311,7 +3338,7 @@
       <c r="G7" s="12">
         <v>65</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="23">
         <f t="shared" si="0"/>
         <v>261.89082713498442</v>
       </c>
@@ -3322,18 +3349,18 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B8" s="12">
         <v>1.75</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="29">
         <v>64.900000000000006</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="22">
         <v>0.5</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="22">
         <v>1.24</v>
       </c>
       <c r="F8" s="12">
@@ -3342,7 +3369,7 @@
       <c r="G8" s="12">
         <v>60</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="23">
         <f t="shared" si="0"/>
         <v>167.6418097083822</v>
       </c>
@@ -3354,422 +3381,422 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
-      <c r="H9" s="24"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
-      <c r="H10" s="24"/>
+      <c r="H10" s="23"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
-      <c r="H11" s="24"/>
+      <c r="H11" s="23"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
-      <c r="H12" s="24"/>
+      <c r="H12" s="23"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
-      <c r="H13" s="24"/>
+      <c r="H13" s="23"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
-      <c r="H14" s="24"/>
+      <c r="H14" s="23"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="23"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
-      <c r="H16" s="24"/>
+      <c r="H16" s="23"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
-      <c r="H17" s="24"/>
+      <c r="H17" s="23"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
-      <c r="H18" s="24"/>
+      <c r="H18" s="23"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
-      <c r="H19" s="24"/>
+      <c r="H19" s="23"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
-      <c r="H20" s="24"/>
+      <c r="H20" s="23"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
-      <c r="H21" s="24"/>
+      <c r="H21" s="23"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
-      <c r="H22" s="24"/>
+      <c r="H22" s="23"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
-      <c r="H23" s="24"/>
+      <c r="H23" s="23"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
-      <c r="H24" s="24"/>
+      <c r="H24" s="23"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
-      <c r="H25" s="24"/>
+      <c r="H25" s="23"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
-      <c r="H26" s="24"/>
+      <c r="H26" s="23"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
-      <c r="H27" s="24"/>
+      <c r="H27" s="23"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
-      <c r="H28" s="24"/>
+      <c r="H28" s="23"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
-      <c r="H29" s="24"/>
+      <c r="H29" s="23"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
-      <c r="H30" s="24"/>
+      <c r="H30" s="23"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="12"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
-      <c r="H31" s="25"/>
+      <c r="H31" s="24"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
-      <c r="H32" s="25"/>
+      <c r="H32" s="24"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="12"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
       <c r="F33" s="12"/>
       <c r="G33" s="12"/>
-      <c r="H33" s="25"/>
+      <c r="H33" s="24"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="12"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
-      <c r="H34" s="25"/>
+      <c r="H34" s="24"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="B35" s="12"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
-      <c r="H35" s="25"/>
+      <c r="H35" s="24"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="B36" s="12"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
-      <c r="H36" s="25"/>
+      <c r="H36" s="24"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
-      <c r="H37" s="25"/>
+      <c r="H37" s="24"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
       <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="23"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="22"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12"/>
-      <c r="H38" s="25"/>
+      <c r="H38" s="24"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
+      <c r="C39" s="30"/>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
       <c r="G39" s="12"/>
-      <c r="H39" s="25"/>
+      <c r="H39" s="24"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
+      <c r="C40" s="30"/>
       <c r="D40" s="12"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
       <c r="G40" s="12"/>
-      <c r="H40" s="25"/>
+      <c r="H40" s="24"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
       <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
+      <c r="C41" s="30"/>
       <c r="D41" s="12"/>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
       <c r="G41" s="12"/>
-      <c r="H41" s="25"/>
+      <c r="H41" s="24"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
       <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
+      <c r="C42" s="30"/>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>
-      <c r="H42" s="25"/>
+      <c r="H42" s="24"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
+      <c r="C43" s="30"/>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
-      <c r="H43" s="25"/>
+      <c r="H43" s="24"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
+      <c r="C44" s="30"/>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
-      <c r="H44" s="25"/>
+      <c r="H44" s="24"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
+      <c r="C45" s="30"/>
       <c r="D45" s="12"/>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
-      <c r="H45" s="25"/>
+      <c r="H45" s="24"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
+      <c r="C46" s="30"/>
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
-      <c r="H46" s="25"/>
+      <c r="H46" s="24"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
+      <c r="C47" s="30"/>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
       <c r="G47" s="12"/>
-      <c r="H47" s="25"/>
+      <c r="H47" s="24"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
+      <c r="C48" s="30"/>
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
       <c r="F48" s="12"/>
       <c r="G48" s="12"/>
-      <c r="H48" s="25"/>
+      <c r="H48" s="24"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
-      <c r="C49" s="12"/>
+      <c r="C49" s="30"/>
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
-      <c r="H49" s="25"/>
+      <c r="H49" s="24"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="12"/>
       <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
+      <c r="C50" s="30"/>
       <c r="D50" s="12"/>
       <c r="E50" s="12"/>
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
-      <c r="H50" s="25"/>
+      <c r="H50" s="24"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I38">
@@ -3787,25 +3814,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="12">
-        <v>0.26</v>
+        <v>0.09</v>
       </c>
       <c r="C2" s="4" t="str">
         <f>B5&amp;"/kWh"</f>
-        <v>€/kWh</v>
+        <v>$/kWh</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3817,26 +3844,26 @@
       </c>
       <c r="C3" s="4" t="str">
         <f>B5&amp;"/h"</f>
-        <v>€/h</v>
+        <v>$/h</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="12">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="28" t="s">
-        <v>16</v>
+      <c r="B5" s="27" t="s">
+        <v>67</v>
       </c>
       <c r="C5" s="4"/>
     </row>

</xml_diff>